<commit_message>
Added corrections and points
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29E9F1D-E2DB-4EB4-95FC-9C9156AB04CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0885AF-AD7C-4A37-91B9-C5699E77D523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="4860" windowWidth="19420" windowHeight="10420" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Group Members</t>
-  </si>
-  <si>
-    <t>Project</t>
   </si>
   <si>
     <t>Achieved Points</t>
@@ -119,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -249,21 +246,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -272,21 +254,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -323,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -334,15 +301,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -660,7 +625,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -675,8 +640,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
-        <v>10</v>
+      <c r="A1" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -702,39 +667,39 @@
       <c r="W1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="5"/>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="16">
+        <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
+        <v>2</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="18">
-        <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="16">
+        <f>SUM(B6,C6,D6,E6,F6,G6:H6,I6,J6,K6,L6,M6,N6)</f>
+        <v>39</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="18">
-        <f>SUM(B6,C6,D6,E6,F6,G6:H6,I6,J6,K6,L6,M6,N6)</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="18" t="e">
+      <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>#DIV/0!</v>
+        <v>5.128205128205128E-2</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -773,45 +738,45 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="15">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="15">
-        <v>3</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="C4" s="13">
+        <v>3</v>
+      </c>
+      <c r="D4" s="13">
         <v>4</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="13">
         <v>5</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <v>6</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="13">
         <v>7</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="13">
         <v>8</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <v>9</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="13">
         <v>10</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="13">
         <v>11</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="13">
         <v>12</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="13">
         <v>13</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="14">
         <v>14</v>
       </c>
       <c r="O4" s="3"/>
@@ -825,22 +790,48 @@
       <c r="W4" s="3"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="14"/>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -853,21 +844,47 @@
     </row>
     <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3</v>
+      </c>
+      <c r="E6" s="9">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8">
+        <v>3</v>
+      </c>
+      <c r="G6" s="9">
+        <v>3</v>
+      </c>
+      <c r="H6" s="8">
+        <v>3</v>
+      </c>
+      <c r="I6" s="9">
+        <v>3</v>
+      </c>
+      <c r="J6" s="8">
+        <v>3</v>
+      </c>
+      <c r="K6" s="9">
+        <v>3</v>
+      </c>
+      <c r="L6" s="8">
+        <v>3</v>
+      </c>
+      <c r="M6" s="9">
+        <v>3</v>
+      </c>
+      <c r="N6" s="8">
+        <v>3</v>
+      </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -878,7 +895,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -904,20 +921,48 @@
       <c r="W7" s="3"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13">
+        <v>2</v>
+      </c>
+      <c r="C8" s="13">
+        <v>3</v>
+      </c>
+      <c r="D8" s="13">
+        <v>4</v>
+      </c>
+      <c r="E8" s="13">
+        <v>5</v>
+      </c>
+      <c r="F8" s="13">
+        <v>6</v>
+      </c>
+      <c r="G8" s="13">
+        <v>7</v>
+      </c>
+      <c r="H8" s="13">
+        <v>8</v>
+      </c>
+      <c r="I8" s="13">
+        <v>9</v>
+      </c>
+      <c r="J8" s="13">
+        <v>10</v>
+      </c>
+      <c r="K8" s="13">
+        <v>11</v>
+      </c>
+      <c r="L8" s="13">
+        <v>12</v>
+      </c>
+      <c r="M8" s="13">
+        <v>13</v>
+      </c>
+      <c r="N8" s="14">
+        <v>14</v>
+      </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
@@ -928,20 +973,48 @@
       <c r="W8" s="3"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="A9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -952,21 +1025,49 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+    <row r="10" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9">
+        <v>3</v>
+      </c>
+      <c r="F10" s="8">
+        <v>3</v>
+      </c>
+      <c r="G10" s="9">
+        <v>3</v>
+      </c>
+      <c r="H10" s="8">
+        <v>3</v>
+      </c>
+      <c r="I10" s="9">
+        <v>3</v>
+      </c>
+      <c r="J10" s="8">
+        <v>3</v>
+      </c>
+      <c r="K10" s="9">
+        <v>3</v>
+      </c>
+      <c r="L10" s="8">
+        <v>3</v>
+      </c>
+      <c r="M10" s="9">
+        <v>3</v>
+      </c>
+      <c r="N10" s="8">
+        <v>3</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -977,7 +1078,7 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1003,20 +1104,48 @@
       <c r="W11" s="3"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="A12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="13">
+        <v>2</v>
+      </c>
+      <c r="C12" s="13">
+        <v>3</v>
+      </c>
+      <c r="D12" s="13">
+        <v>4</v>
+      </c>
+      <c r="E12" s="13">
+        <v>5</v>
+      </c>
+      <c r="F12" s="13">
+        <v>6</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13">
+        <v>8</v>
+      </c>
+      <c r="I12" s="13">
+        <v>9</v>
+      </c>
+      <c r="J12" s="13">
+        <v>10</v>
+      </c>
+      <c r="K12" s="13">
+        <v>11</v>
+      </c>
+      <c r="L12" s="13">
+        <v>12</v>
+      </c>
+      <c r="M12" s="13">
+        <v>13</v>
+      </c>
+      <c r="N12" s="14">
+        <v>14</v>
+      </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1028,20 +1157,48 @@
       <c r="W12" s="3"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="A13" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -1052,21 +1209,49 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+    <row r="14" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9">
+        <v>3</v>
+      </c>
+      <c r="D14" s="8">
+        <v>3</v>
+      </c>
+      <c r="E14" s="9">
+        <v>3</v>
+      </c>
+      <c r="F14" s="8">
+        <v>3</v>
+      </c>
+      <c r="G14" s="9">
+        <v>3</v>
+      </c>
+      <c r="H14" s="8">
+        <v>3</v>
+      </c>
+      <c r="I14" s="9">
+        <v>3</v>
+      </c>
+      <c r="J14" s="8">
+        <v>3</v>
+      </c>
+      <c r="K14" s="9">
+        <v>3</v>
+      </c>
+      <c r="L14" s="8">
+        <v>3</v>
+      </c>
+      <c r="M14" s="9">
+        <v>3</v>
+      </c>
+      <c r="N14" s="8">
+        <v>3</v>
+      </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>

</xml_diff>

<commit_message>
Added corrections for exercise 3
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0885AF-AD7C-4A37-91B9-C5699E77D523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB55CC6-3DE0-4E5B-AEE3-73B7F2C8E2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="4860" windowWidth="19420" windowHeight="10420" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -625,7 +625,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,7 +685,7 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
@@ -699,7 +699,7 @@
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>5.128205128205128E-2</v>
+        <v>0.12820512820512819</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -797,7 +797,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -980,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -1164,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Added corrections and point for exercise 4
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB55CC6-3DE0-4E5B-AEE3-73B7F2C8E2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1851C067-C416-40B3-9294-74547B77DF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -625,7 +625,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,7 +685,7 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
@@ -699,7 +699,7 @@
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>0.12820512820512819</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -800,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -983,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -1167,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Added corrections and point for exercise 5
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1851C067-C416-40B3-9294-74547B77DF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A743F3BB-F031-4848-88CB-16F2138364A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -625,7 +625,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,7 +685,7 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
@@ -699,7 +699,7 @@
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>0.15384615384615385</v>
+        <v>0.17948717948717949</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -803,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -986,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1170,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Added corrections and point for exercise 6
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A743F3BB-F031-4848-88CB-16F2138364A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D6BA52-9408-4901-BF92-44586752B971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -625,7 +625,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,7 +685,7 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
@@ -699,7 +699,7 @@
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>0.17948717948717949</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -806,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -989,7 +989,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -1173,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Added corrections for exercise 7
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D6BA52-9408-4901-BF92-44586752B971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF197ED-9516-472C-A6C3-15C823D33129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619DA100-CC06-463D-8753-D40F02816899}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added corrections for exercise 8
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF197ED-9516-472C-A6C3-15C823D33129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A5F8D3-24EF-4794-8C8B-4E4A29D8A60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -625,7 +617,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="W5" activeCellId="1" sqref="U10 W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,7 +677,7 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
@@ -699,7 +691,7 @@
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>0.23076923076923078</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -812,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -995,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
@@ -1179,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Added corrections for exercise 9
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A5F8D3-24EF-4794-8C8B-4E4A29D8A60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5816C3B2-331F-4918-89EA-D6CDD1DB95E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
+    <workbookView xWindow="-19310" yWindow="4860" windowWidth="19420" windowHeight="10420" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619DA100-CC06-463D-8753-D40F02816899}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W5" activeCellId="1" sqref="U10 W5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -677,21 +677,21 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="16">
         <f>SUM(B6,C6,D6,E6,F6,G6:H6,I6,J6,K6,L6,M6,N6)</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>0.30769230769230771</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -768,9 +768,7 @@
       <c r="M4" s="13">
         <v>13</v>
       </c>
-      <c r="N4" s="14">
-        <v>14</v>
-      </c>
+      <c r="N4" s="14"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -807,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
@@ -821,9 +819,7 @@
       <c r="M5" s="2">
         <v>0</v>
       </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
+      <c r="N5" s="1"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -874,9 +870,7 @@
       <c r="M6" s="9">
         <v>3</v>
       </c>
-      <c r="N6" s="8">
-        <v>3</v>
-      </c>
+      <c r="N6" s="8"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -952,9 +946,7 @@
       <c r="M8" s="13">
         <v>13</v>
       </c>
-      <c r="N8" s="14">
-        <v>14</v>
-      </c>
+      <c r="N8" s="14"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
@@ -990,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="I9" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -1004,9 +996,7 @@
       <c r="M9" s="2">
         <v>0</v>
       </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
+      <c r="N9" s="1"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -1057,9 +1047,7 @@
       <c r="M10" s="9">
         <v>3</v>
       </c>
-      <c r="N10" s="8">
-        <v>3</v>
-      </c>
+      <c r="N10" s="8"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -1135,9 +1123,7 @@
       <c r="M12" s="13">
         <v>13</v>
       </c>
-      <c r="N12" s="14">
-        <v>14</v>
-      </c>
+      <c r="N12" s="14"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1174,7 +1160,7 @@
         <v>3</v>
       </c>
       <c r="I13" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
@@ -1188,9 +1174,7 @@
       <c r="M13" s="2">
         <v>0</v>
       </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
+      <c r="N13" s="1"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -1241,9 +1225,7 @@
       <c r="M14" s="9">
         <v>3</v>
       </c>
-      <c r="N14" s="8">
-        <v>3</v>
-      </c>
+      <c r="N14" s="8"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>

</xml_diff>

<commit_message>
Added corrections for exercise 10
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5816C3B2-331F-4918-89EA-D6CDD1DB95E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61250ADB-746A-40E6-A993-07C1CF893B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="4860" windowWidth="19420" windowHeight="10420" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -617,7 +628,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -677,7 +688,7 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
@@ -691,7 +702,7 @@
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>0.41666666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -808,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
@@ -985,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -1163,7 +1174,7 @@
         <v>3</v>
       </c>
       <c r="J13" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Added corrections for exercise 11
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61250ADB-746A-40E6-A993-07C1CF893B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0723B3A-4622-463D-A7F5-69403452924D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="4860" windowWidth="19420" windowHeight="10420" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -617,7 +606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,7 +617,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -688,7 +677,7 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
@@ -702,7 +691,7 @@
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -822,7 +811,7 @@
         <v>3</v>
       </c>
       <c r="K5" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
@@ -999,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="K9" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L9" s="1">
         <v>0</v>
@@ -1177,7 +1166,7 @@
         <v>3</v>
       </c>
       <c r="K13" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Added corrections for exercise 12
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0723B3A-4622-463D-A7F5-69403452924D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448C80BB-0350-4387-A2D2-5EA3771411EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="4860" windowWidth="19420" windowHeight="10420" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -606,7 +615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -616,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619DA100-CC06-463D-8753-D40F02816899}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -677,7 +686,7 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
@@ -691,7 +700,7 @@
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>0.58333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -814,7 +823,7 @@
         <v>3</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M5" s="2">
         <v>0</v>
@@ -991,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="L9" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M9" s="2">
         <v>0</v>
@@ -1169,7 +1178,7 @@
         <v>3</v>
       </c>
       <c r="L13" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Added corrections for exercise 13
</commit_message>
<xml_diff>
--- a/group2.xlsx
+++ b/group2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Hendrik_Daten\Uni\Master\Bildverarbeitung\Arbeit\GruppenRepos\Gruppe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448C80BB-0350-4387-A2D2-5EA3771411EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E361B219-8302-49A9-A0BF-B3A4C71B78A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="4860" windowWidth="19420" windowHeight="10420" xr2:uid="{8A91DCA3-4ECC-4D68-AFAE-4BAC306754D3}"/>
   </bookViews>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -625,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619DA100-CC06-463D-8753-D40F02816899}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,7 +677,7 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(B5,C5,D5,E5,F5,G5:H5,I5,J5,K5,L5,M5,N5)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>4</v>
@@ -700,7 +691,7 @@
       </c>
       <c r="N2" s="16">
         <f>H2/K2</f>
-        <v>0.66666666666666663</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -826,7 +817,7 @@
         <v>3</v>
       </c>
       <c r="M5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="3"/>
@@ -1003,7 +994,7 @@
         <v>3</v>
       </c>
       <c r="M9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="3"/>
@@ -1181,7 +1172,7 @@
         <v>3</v>
       </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="3"/>

</xml_diff>